<commit_message>
test hypothesiswith data excel updated
</commit_message>
<xml_diff>
--- a/Test Hypothesis WIth Data/AdvancedTestHypothesis/New Microsoft Excel Worksheet.xlsx
+++ b/Test Hypothesis WIth Data/AdvancedTestHypothesis/New Microsoft Excel Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,8 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="67">
   <si>
     <t>A</t>
   </si>
@@ -205,6 +207,27 @@
   </si>
   <si>
     <t>100 </t>
+  </si>
+  <si>
+    <t>Drug A</t>
+  </si>
+  <si>
+    <t>Drug B</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>Low sound</t>
+  </si>
+  <si>
+    <t>High sound</t>
   </si>
 </sst>
 </file>
@@ -369,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -385,9 +408,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -406,6 +426,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,30 +735,30 @@
     </row>
     <row r="2" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="5"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="O2" s="5"/>
@@ -739,18 +767,18 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
       <c r="H3" s="6"/>
       <c r="J3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="3:15" ht="30" x14ac:dyDescent="0.25">
@@ -870,12 +898,12 @@
       </c>
     </row>
     <row r="10" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L11" s="9" t="s">
+      <c r="L11" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -884,37 +912,37 @@
         <f>CHITEST(D4:G5,K4:N5)</f>
         <v>0.16197005772379947</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L12" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L13" s="9" t="s">
+      <c r="L13" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L14" s="9" t="s">
+      <c r="L14" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L16" s="9" t="s">
+      <c r="L16" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="12:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L17" s="9" t="s">
+      <c r="L17" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="12:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L18" s="9" t="s">
+      <c r="L18" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1077,242 +1105,242 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="10">
-        <v>4</v>
-      </c>
-      <c r="L16" s="10">
-        <v>4</v>
-      </c>
-      <c r="M16" s="10">
-        <v>4</v>
-      </c>
-      <c r="N16" s="10">
+      <c r="K16" s="9">
+        <v>4</v>
+      </c>
+      <c r="L16" s="9">
+        <v>4</v>
+      </c>
+      <c r="M16" s="9">
+        <v>4</v>
+      </c>
+      <c r="N16" s="9">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="9">
         <v>12.5</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="9">
         <v>14.400000000000002</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="9">
         <v>14.299999999999999</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="9">
         <v>41.199999999999996</v>
       </c>
     </row>
     <row r="18" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="9">
         <v>3.125</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="9">
         <v>3.6000000000000005</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="9">
         <v>3.5749999999999997</v>
       </c>
-      <c r="N18" s="10">
+      <c r="N18" s="9">
         <v>3.4333333333333331</v>
       </c>
     </row>
     <row r="19" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="9">
         <v>0.1158333333333334</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="9">
         <v>8.6666666666666614E-2</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="9">
         <v>0.15583333333333327</v>
       </c>
-      <c r="N19" s="10">
+      <c r="N19" s="9">
         <v>0.14969696969697308</v>
       </c>
     </row>
     <row r="20" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
     </row>
     <row r="21" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J21" s="11" t="s">
+      <c r="J21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
     </row>
     <row r="22" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="10">
-        <v>4</v>
-      </c>
-      <c r="L22" s="10">
-        <v>4</v>
-      </c>
-      <c r="M22" s="10">
-        <v>4</v>
-      </c>
-      <c r="N22" s="10">
+      <c r="K22" s="9">
+        <v>4</v>
+      </c>
+      <c r="L22" s="9">
+        <v>4</v>
+      </c>
+      <c r="M22" s="9">
+        <v>4</v>
+      </c>
+      <c r="N22" s="9">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J23" s="10" t="s">
+      <c r="J23" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="9">
         <v>11.5</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="9">
         <v>14.5</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="9">
         <v>15</v>
       </c>
-      <c r="N23" s="10">
+      <c r="N23" s="9">
         <v>40.999999999999993</v>
       </c>
     </row>
     <row r="24" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="9">
         <v>2.875</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="9">
         <v>3.625</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="9">
         <v>3.75</v>
       </c>
-      <c r="N24" s="10">
+      <c r="N24" s="9">
         <v>3.4166666666666661</v>
       </c>
     </row>
     <row r="25" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="9">
         <v>0.1824999999999998</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25" s="9">
         <v>0.19583333333333286</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="9">
         <v>9.6666666666666581E-2</v>
       </c>
-      <c r="N25" s="10">
+      <c r="N25" s="9">
         <v>0.2924242424242452</v>
       </c>
     </row>
     <row r="26" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
     </row>
     <row r="27" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J27" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
+      <c r="J27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
     </row>
     <row r="28" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J28" s="10" t="s">
+      <c r="J28" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="9">
         <v>8</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28" s="9">
         <v>8</v>
       </c>
-      <c r="M28" s="10">
+      <c r="M28" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J29" s="10" t="s">
+      <c r="J29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="9">
         <v>24</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L29" s="9">
         <v>28.900000000000002</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="9">
         <v>29.299999999999997</v>
       </c>
     </row>
     <row r="30" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J30" s="10" t="s">
+      <c r="J30" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K30" s="10">
+      <c r="K30" s="9">
         <v>3</v>
       </c>
-      <c r="L30" s="10">
+      <c r="L30" s="9">
         <v>3.6125000000000003</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M30" s="9">
         <v>3.6624999999999996</v>
       </c>
     </row>
     <row r="31" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J31" s="10" t="s">
+      <c r="J31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K31" s="9">
         <v>0.14571428571428516</v>
       </c>
-      <c r="L31" s="10">
+      <c r="L31" s="9">
         <v>0.12124999999999993</v>
       </c>
-      <c r="M31" s="10">
+      <c r="M31" s="9">
         <v>0.11696428571428563</v>
       </c>
     </row>
     <row r="32" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
     </row>
     <row r="34" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J34" t="s">
@@ -1320,137 +1348,137 @@
       </c>
     </row>
     <row r="35" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J35" s="13" t="s">
+      <c r="J35" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K35" s="13" t="s">
+      <c r="K35" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="L35" s="13" t="s">
+      <c r="L35" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="M35" s="13" t="s">
+      <c r="M35" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="N35" s="13" t="s">
+      <c r="N35" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="O35" s="13" t="s">
+      <c r="O35" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="P35" s="13" t="s">
+      <c r="P35" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="36" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J36" s="10" t="s">
+      <c r="J36" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K36" s="9">
         <v>1.6666666666669272E-3</v>
       </c>
-      <c r="L36" s="10">
+      <c r="L36" s="9">
         <v>1</v>
       </c>
-      <c r="M36" s="10">
+      <c r="M36" s="9">
         <v>1.6666666666669272E-3</v>
       </c>
-      <c r="N36" s="10">
+      <c r="N36" s="9">
         <v>1.2000000000001877E-2</v>
       </c>
-      <c r="O36" s="10">
+      <c r="O36" s="9">
         <v>0.91398265748428698</v>
       </c>
-      <c r="P36" s="10">
+      <c r="P36" s="9">
         <v>4.4138734191705664</v>
       </c>
     </row>
     <row r="37" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J37" s="10" t="s">
+      <c r="J37" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="K37" s="10">
+      <c r="K37" s="9">
         <v>2.1775000000000007</v>
       </c>
-      <c r="L37" s="10">
+      <c r="L37" s="9">
         <v>2</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M37" s="9">
         <v>1.0887500000000003</v>
       </c>
-      <c r="N37" s="10">
+      <c r="N37" s="9">
         <v>7.839000000000004</v>
       </c>
-      <c r="O37" s="10">
+      <c r="O37" s="9">
         <v>3.559064941048024E-3</v>
       </c>
-      <c r="P37" s="10">
+      <c r="P37" s="9">
         <v>3.5545571456617879</v>
       </c>
     </row>
     <row r="38" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J38" s="10" t="s">
+      <c r="J38" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K38" s="10">
+      <c r="K38" s="9">
         <v>0.18583333333333307</v>
       </c>
-      <c r="L38" s="10">
+      <c r="L38" s="9">
         <v>2</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M38" s="9">
         <v>9.2916666666666536E-2</v>
       </c>
-      <c r="N38" s="10">
+      <c r="N38" s="9">
         <v>0.66899999999999915</v>
       </c>
-      <c r="O38" s="10">
+      <c r="O38" s="9">
         <v>0.52450368392211755</v>
       </c>
-      <c r="P38" s="10">
+      <c r="P38" s="9">
         <v>3.5545571456617879</v>
       </c>
     </row>
     <row r="39" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J39" s="10" t="s">
+      <c r="J39" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K39" s="10">
+      <c r="K39" s="9">
         <v>2.4999999999999996</v>
       </c>
-      <c r="L39" s="10">
+      <c r="L39" s="9">
         <v>18</v>
       </c>
-      <c r="M39" s="10">
+      <c r="M39" s="9">
         <v>0.13888888888888887</v>
       </c>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
     </row>
     <row r="40" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
     </row>
     <row r="41" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J41" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K41" s="12">
+      <c r="J41" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" s="11">
         <v>4.8650000000000002</v>
       </c>
-      <c r="L41" s="12">
+      <c r="L41" s="11">
         <v>23</v>
       </c>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="12"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1754,12 +1782,12 @@
       <c r="C10">
         <v>902</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -1768,16 +1796,16 @@
       <c r="C11">
         <v>919</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="10">
-        <v>4</v>
-      </c>
-      <c r="J11" s="10">
-        <v>4</v>
-      </c>
-      <c r="K11" s="10">
+      <c r="I11" s="9">
+        <v>4</v>
+      </c>
+      <c r="J11" s="9">
+        <v>4</v>
+      </c>
+      <c r="K11" s="9">
         <v>8</v>
       </c>
     </row>
@@ -1788,16 +1816,16 @@
       <c r="C12">
         <v>919</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <v>3411</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="9">
         <v>3622</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <v>7033</v>
       </c>
     </row>
@@ -1808,246 +1836,246 @@
       <c r="C13">
         <v>900</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <v>852.75</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <v>905.5</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <v>879.125</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="9">
         <v>660.91666666666663</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="9">
         <v>193.66666666666666</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="9">
         <v>1161.2678571428571</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
     </row>
     <row r="17" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="10">
-        <v>4</v>
-      </c>
-      <c r="J17" s="10">
-        <v>4</v>
-      </c>
-      <c r="K17" s="10">
+      <c r="I17" s="9">
+        <v>4</v>
+      </c>
+      <c r="J17" s="9">
+        <v>4</v>
+      </c>
+      <c r="K17" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="9">
         <v>3207</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="9">
         <v>3243</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="9">
         <v>6450</v>
       </c>
     </row>
     <row r="19" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="9">
         <v>801.75</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="9">
         <v>810.75</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="9">
         <v>806.25</v>
       </c>
     </row>
     <row r="20" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="9">
         <v>81.583333333333329</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="9">
         <v>62.916666666666664</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="9">
         <v>85.071428571428569</v>
       </c>
     </row>
     <row r="21" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="8:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
     </row>
     <row r="23" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="10">
-        <v>4</v>
-      </c>
-      <c r="J23" s="10">
-        <v>4</v>
-      </c>
-      <c r="K23" s="10">
+      <c r="I23" s="9">
+        <v>4</v>
+      </c>
+      <c r="J23" s="9">
+        <v>4</v>
+      </c>
+      <c r="K23" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="9">
         <v>3620</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="9">
         <v>3640</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="9">
         <v>7260</v>
       </c>
     </row>
     <row r="25" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="9">
         <v>905</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="9">
         <v>910</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="9">
         <v>907.5</v>
       </c>
     </row>
     <row r="26" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="9">
         <v>80.666666666666671</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="9">
         <v>108.66666666666667</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="9">
         <v>88.285714285714292</v>
       </c>
     </row>
     <row r="27" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
     </row>
     <row r="28" spans="8:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H28" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
+      <c r="H28" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
     </row>
     <row r="29" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="9">
         <v>12</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J29" s="9">
         <v>12</v>
       </c>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
     </row>
     <row r="30" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H30" s="10" t="s">
+      <c r="H30" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I30" s="9">
         <v>10238</v>
       </c>
-      <c r="J30" s="10">
+      <c r="J30" s="9">
         <v>10505</v>
       </c>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
     </row>
     <row r="31" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="9">
         <v>853.16666666666663</v>
       </c>
-      <c r="J31" s="10">
+      <c r="J31" s="9">
         <v>875.41666666666663</v>
       </c>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
     </row>
     <row r="32" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="9">
         <v>2162.878787878788</v>
       </c>
-      <c r="J32" s="10">
+      <c r="J32" s="9">
         <v>2384.265151515152</v>
       </c>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
     </row>
     <row r="33" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
     </row>
     <row r="35" spans="8:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H35" t="s">
@@ -2055,137 +2083,137 @@
       </c>
     </row>
     <row r="36" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="I36" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="J36" s="13" t="s">
+      <c r="J36" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="K36" s="13" t="s">
+      <c r="K36" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L36" s="13" t="s">
+      <c r="L36" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="M36" s="13" t="s">
+      <c r="M36" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="N36" s="13" t="s">
+      <c r="N36" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H37" s="10" t="s">
+      <c r="H37" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I37" s="10">
+      <c r="I37" s="9">
         <v>43646.583333333336</v>
       </c>
-      <c r="J37" s="10">
+      <c r="J37" s="9">
         <v>2</v>
       </c>
-      <c r="K37" s="10">
+      <c r="K37" s="9">
         <v>21823.291666666668</v>
       </c>
-      <c r="L37" s="10">
+      <c r="L37" s="9">
         <v>110.1800014024262</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M37" s="9">
         <v>7.9864193282714261E-11</v>
       </c>
-      <c r="N37" s="10">
+      <c r="N37" s="9">
         <v>3.5545571456617879</v>
       </c>
     </row>
     <row r="38" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H38" s="10" t="s">
+      <c r="H38" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I38" s="9">
         <v>2970.3749999999927</v>
       </c>
-      <c r="J38" s="10">
+      <c r="J38" s="9">
         <v>1</v>
       </c>
-      <c r="K38" s="10">
+      <c r="K38" s="9">
         <v>2970.3749999999927</v>
       </c>
-      <c r="L38" s="10">
+      <c r="L38" s="9">
         <v>14.99663417712639</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M38" s="9">
         <v>1.1156188522220929E-3</v>
       </c>
-      <c r="N38" s="10">
+      <c r="N38" s="9">
         <v>4.4138734191705664</v>
       </c>
     </row>
     <row r="39" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H39" s="10" t="s">
+      <c r="H39" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I39" s="10">
+      <c r="I39" s="9">
         <v>2806.7500000000073</v>
       </c>
-      <c r="J39" s="10">
+      <c r="J39" s="9">
         <v>2</v>
       </c>
-      <c r="K39" s="10">
+      <c r="K39" s="9">
         <v>1403.3750000000036</v>
       </c>
-      <c r="L39" s="10">
+      <c r="L39" s="9">
         <v>7.0852675127971567</v>
       </c>
-      <c r="M39" s="10">
+      <c r="M39" s="9">
         <v>5.3743753282750988E-3</v>
       </c>
-      <c r="N39" s="10">
+      <c r="N39" s="9">
         <v>3.5545571456617879</v>
       </c>
     </row>
     <row r="40" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H40" s="10" t="s">
+      <c r="H40" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I40" s="10">
+      <c r="I40" s="9">
         <v>3565.25</v>
       </c>
-      <c r="J40" s="10">
+      <c r="J40" s="9">
         <v>18</v>
       </c>
-      <c r="K40" s="10">
+      <c r="K40" s="9">
         <v>198.06944444444446</v>
       </c>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
     </row>
     <row r="41" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
     </row>
     <row r="42" spans="8:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H42" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I42" s="12">
+      <c r="H42" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" s="11">
         <v>52988.958333333336</v>
       </c>
-      <c r="J42" s="12">
+      <c r="J42" s="11">
         <v>23</v>
       </c>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2220,7 +2248,7 @@
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <v>19.5</v>
       </c>
     </row>
@@ -2242,7 +2270,7 @@
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="14">
+      <c r="K7" s="13">
         <v>18</v>
       </c>
     </row>
@@ -2266,7 +2294,7 @@
         <v>17</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="14">
+      <c r="K8" s="13">
         <v>18</v>
       </c>
     </row>
@@ -2292,7 +2320,7 @@
       <c r="J9" s="4">
         <v>14</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="14">
         <v>16.66</v>
       </c>
     </row>
@@ -2402,12 +2430,12 @@
       <c r="D10">
         <v>801</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C11">
@@ -2416,16 +2444,16 @@
       <c r="D11">
         <v>809</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="10">
-        <v>4</v>
-      </c>
-      <c r="J11" s="10">
-        <v>4</v>
-      </c>
-      <c r="K11" s="10">
+      <c r="I11" s="9">
+        <v>4</v>
+      </c>
+      <c r="J11" s="9">
+        <v>4</v>
+      </c>
+      <c r="K11" s="9">
         <v>8</v>
       </c>
     </row>
@@ -2439,16 +2467,16 @@
       <c r="D12">
         <v>902</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <v>3411</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="9">
         <v>3622</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <v>7033</v>
       </c>
     </row>
@@ -2459,16 +2487,16 @@
       <c r="D13">
         <v>919</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <v>852.75</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <v>905.5</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <v>879.125</v>
       </c>
     </row>
@@ -2479,16 +2507,16 @@
       <c r="D14">
         <v>919</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="9">
         <v>660.91666666666663</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="9">
         <v>193.66666666666666</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="9">
         <v>1161.2678571428571</v>
       </c>
     </row>
@@ -2499,218 +2527,218 @@
       <c r="D15">
         <v>900</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
     </row>
     <row r="17" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="10">
-        <v>4</v>
-      </c>
-      <c r="J17" s="10">
-        <v>4</v>
-      </c>
-      <c r="K17" s="10">
+      <c r="I17" s="9">
+        <v>4</v>
+      </c>
+      <c r="J17" s="9">
+        <v>4</v>
+      </c>
+      <c r="K17" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="9">
         <v>3207</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="9">
         <v>3243</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="9">
         <v>6450</v>
       </c>
     </row>
     <row r="19" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="9">
         <v>801.75</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="9">
         <v>810.75</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="9">
         <v>806.25</v>
       </c>
     </row>
     <row r="20" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="9">
         <v>81.583333333333329</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="9">
         <v>62.916666666666664</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="9">
         <v>85.071428571428569</v>
       </c>
     </row>
     <row r="21" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="8:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
     </row>
     <row r="23" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="10">
-        <v>4</v>
-      </c>
-      <c r="J23" s="10">
-        <v>4</v>
-      </c>
-      <c r="K23" s="10">
+      <c r="I23" s="9">
+        <v>4</v>
+      </c>
+      <c r="J23" s="9">
+        <v>4</v>
+      </c>
+      <c r="K23" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="9">
         <v>3620</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="9">
         <v>3640</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="9">
         <v>7260</v>
       </c>
     </row>
     <row r="25" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="9">
         <v>905</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="9">
         <v>910</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="9">
         <v>907.5</v>
       </c>
     </row>
     <row r="26" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="9">
         <v>80.666666666666671</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="9">
         <v>108.66666666666667</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="9">
         <v>88.285714285714292</v>
       </c>
     </row>
     <row r="27" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
     </row>
     <row r="28" spans="8:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H28" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
+      <c r="H28" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
     </row>
     <row r="29" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="9">
         <v>12</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J29" s="9">
         <v>12</v>
       </c>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
     </row>
     <row r="30" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H30" s="10" t="s">
+      <c r="H30" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I30" s="9">
         <v>10238</v>
       </c>
-      <c r="J30" s="10">
+      <c r="J30" s="9">
         <v>10505</v>
       </c>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
     </row>
     <row r="31" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="9">
         <v>853.16666666666663</v>
       </c>
-      <c r="J31" s="10">
+      <c r="J31" s="9">
         <v>875.41666666666663</v>
       </c>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
     </row>
     <row r="32" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="9">
         <v>2162.878787878788</v>
       </c>
-      <c r="J32" s="10">
+      <c r="J32" s="9">
         <v>2384.265151515152</v>
       </c>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
     </row>
     <row r="33" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
     </row>
     <row r="35" spans="8:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H35" t="s">
@@ -2718,137 +2746,137 @@
       </c>
     </row>
     <row r="36" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="I36" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="J36" s="13" t="s">
+      <c r="J36" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="K36" s="13" t="s">
+      <c r="K36" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L36" s="13" t="s">
+      <c r="L36" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="M36" s="13" t="s">
+      <c r="M36" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="N36" s="13" t="s">
+      <c r="N36" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H37" s="10" t="s">
+      <c r="H37" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I37" s="10">
+      <c r="I37" s="9">
         <v>43646.583333333336</v>
       </c>
-      <c r="J37" s="10">
+      <c r="J37" s="9">
         <v>2</v>
       </c>
-      <c r="K37" s="10">
+      <c r="K37" s="9">
         <v>21823.291666666668</v>
       </c>
-      <c r="L37" s="10">
+      <c r="L37" s="9">
         <v>110.1800014024262</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M37" s="9">
         <v>7.9864193282714261E-11</v>
       </c>
-      <c r="N37" s="10">
+      <c r="N37" s="9">
         <v>3.5545571456617879</v>
       </c>
     </row>
     <row r="38" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H38" s="10" t="s">
+      <c r="H38" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I38" s="9">
         <v>2970.3749999999927</v>
       </c>
-      <c r="J38" s="10">
+      <c r="J38" s="9">
         <v>1</v>
       </c>
-      <c r="K38" s="10">
+      <c r="K38" s="9">
         <v>2970.3749999999927</v>
       </c>
-      <c r="L38" s="10">
+      <c r="L38" s="9">
         <v>14.99663417712639</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M38" s="9">
         <v>1.1156188522220929E-3</v>
       </c>
-      <c r="N38" s="10">
+      <c r="N38" s="9">
         <v>4.4138734191705664</v>
       </c>
     </row>
     <row r="39" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H39" s="10" t="s">
+      <c r="H39" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I39" s="10">
+      <c r="I39" s="9">
         <v>2806.7500000000073</v>
       </c>
-      <c r="J39" s="10">
+      <c r="J39" s="9">
         <v>2</v>
       </c>
-      <c r="K39" s="10">
+      <c r="K39" s="9">
         <v>1403.3750000000036</v>
       </c>
-      <c r="L39" s="10">
+      <c r="L39" s="9">
         <v>7.0852675127971567</v>
       </c>
-      <c r="M39" s="10">
+      <c r="M39" s="9">
         <v>5.3743753282750988E-3</v>
       </c>
-      <c r="N39" s="10">
+      <c r="N39" s="9">
         <v>3.5545571456617879</v>
       </c>
     </row>
     <row r="40" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H40" s="10" t="s">
+      <c r="H40" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I40" s="10">
+      <c r="I40" s="9">
         <v>3565.25</v>
       </c>
-      <c r="J40" s="10">
+      <c r="J40" s="9">
         <v>18</v>
       </c>
-      <c r="K40" s="10">
+      <c r="K40" s="9">
         <v>198.06944444444446</v>
       </c>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
     </row>
     <row r="41" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
     </row>
     <row r="42" spans="8:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H42" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I42" s="12">
+      <c r="H42" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" s="11">
         <v>52988.958333333336</v>
       </c>
-      <c r="J42" s="12">
+      <c r="J42" s="11">
         <v>23</v>
       </c>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2859,13 +2887,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H5">
         <v>0</v>
       </c>
@@ -2876,8 +2904,15 @@
         <f>_xlfn.POISSON.DIST(H5,15,TRUE)</f>
         <v>3.0590232050182579E-7</v>
       </c>
+      <c r="N5" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f>_xlfn.NORM.DIST(100,N11,M11,TRUE)</f>
+        <v>0.58159992812319738</v>
+      </c>
       <c r="H6">
         <v>1</v>
       </c>
@@ -2902,6 +2937,10 @@
       </c>
     </row>
     <row r="9" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f>_xlfn.BINOM.DIST(392,700,0.55,TRUE)</f>
+        <v>0.71528825380610628</v>
+      </c>
       <c r="H9">
         <v>4</v>
       </c>
@@ -2910,6 +2949,10 @@
       </c>
     </row>
     <row r="10" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f>1-E9</f>
+        <v>0.28471174619389372</v>
+      </c>
       <c r="H10">
         <v>5</v>
       </c>
@@ -2917,7 +2960,25 @@
         <v>94</v>
       </c>
     </row>
+    <row r="11" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f>_xlfn.BINOM.DIST(368,500,0.74,TRUE)</f>
+        <v>0.43609604544990754</v>
+      </c>
+      <c r="M11">
+        <f>STDEV(M14:V14)</f>
+        <v>15.103347678945596</v>
+      </c>
+      <c r="N11">
+        <f>AVERAGE(M14:V14)</f>
+        <v>96.888888888888886</v>
+      </c>
+    </row>
     <row r="14" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f>368/500</f>
+        <v>0.73599999999999999</v>
+      </c>
       <c r="M14">
         <v>70</v>
       </c>
@@ -2956,12 +3017,792 @@
       </c>
     </row>
     <row r="18" spans="13:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M18" s="9" t="s">
+      <c r="M18" s="8" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V19"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17:U19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>68</v>
+      </c>
+      <c r="B3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>69</v>
+      </c>
+      <c r="B4">
+        <v>89</v>
+      </c>
+      <c r="M4" s="17">
+        <v>1800</v>
+      </c>
+      <c r="N4" s="18">
+        <v>1200</v>
+      </c>
+      <c r="O4" s="18">
+        <v>1300</v>
+      </c>
+      <c r="P4" s="18">
+        <v>1500</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>1700</v>
+      </c>
+      <c r="R4" s="18">
+        <v>1500</v>
+      </c>
+      <c r="S4" s="18">
+        <v>1200</v>
+      </c>
+      <c r="T4" s="18">
+        <v>1500</v>
+      </c>
+      <c r="U4" s="18">
+        <v>1400</v>
+      </c>
+      <c r="V4" s="18">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>66</v>
+      </c>
+      <c r="B7">
+        <v>74</v>
+      </c>
+      <c r="M7">
+        <f>STDEV(M4:V4)</f>
+        <v>201.10804171997808</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>75</v>
+      </c>
+      <c r="M8" s="18">
+        <f>AVERAGE(M4:V4)</f>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>63</v>
+      </c>
+      <c r="B9">
+        <v>67</v>
+      </c>
+      <c r="M9">
+        <f>_xlfn.NORM.DIST(1500,M8,M7,TRUE)</f>
+        <v>0.61728086827131612</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>71</v>
+      </c>
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="K10">
+        <f>_xlfn.POISSON.DIST(5,3,FALSE)</f>
+        <v>0.10081881344492449</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>73</v>
+      </c>
+      <c r="B11">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <f>BINOMDIST(393,700,0.55,TRUE)</f>
+        <v>0.74053401615361669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>TTEST(A2:A11,B2:B11,2,1)</f>
+        <v>2.7967555151616395E-2</v>
+      </c>
+      <c r="H13">
+        <f>_xlfn.NORM.DIST(186,179,61,TRUE)</f>
+        <v>0.54567998359003544</v>
+      </c>
+      <c r="O13">
+        <f>_xlfn.NORM.DIST(23,20,7,TRUE)</f>
+        <v>0.66588242910237538</v>
+      </c>
+    </row>
+    <row r="17" spans="12:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <f>_xlfn.NORM.DIST(186,179,61,TRUE)</f>
+        <v>0.54567998359003544</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O17" s="4">
+        <v>38</v>
+      </c>
+      <c r="P17" s="4">
+        <v>32</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>54</v>
+      </c>
+      <c r="R17" s="4">
+        <v>50</v>
+      </c>
+      <c r="S17" s="4">
+        <v>33</v>
+      </c>
+      <c r="T17" s="4">
+        <v>43</v>
+      </c>
+      <c r="U17">
+        <f>AVERAGE(O17:T17)</f>
+        <v>41.666666666666664</v>
+      </c>
+    </row>
+    <row r="18" spans="12:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="N18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O18" s="4">
+        <v>49</v>
+      </c>
+      <c r="P18" s="4">
+        <v>36</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>43</v>
+      </c>
+      <c r="R18" s="4">
+        <v>30</v>
+      </c>
+      <c r="S18" s="4">
+        <v>45</v>
+      </c>
+      <c r="T18" s="4">
+        <v>44</v>
+      </c>
+      <c r="U18">
+        <f t="shared" ref="U18:U19" si="0">AVERAGE(O18:T18)</f>
+        <v>41.166666666666664</v>
+      </c>
+    </row>
+    <row r="19" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="N19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O19" s="4">
+        <v>31</v>
+      </c>
+      <c r="P19" s="4">
+        <v>23</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>29</v>
+      </c>
+      <c r="R19" s="4">
+        <v>36</v>
+      </c>
+      <c r="S19" s="4">
+        <v>25</v>
+      </c>
+      <c r="T19" s="4">
+        <v>27</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="0"/>
+        <v>28.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9:P38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="9">
+        <v>4</v>
+      </c>
+      <c r="L13" s="9">
+        <v>4</v>
+      </c>
+      <c r="M13" s="9">
+        <v>4</v>
+      </c>
+      <c r="N13" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="L14" s="9">
+        <v>14.400000000000002</v>
+      </c>
+      <c r="M14" s="9">
+        <v>14.299999999999999</v>
+      </c>
+      <c r="N14" s="9">
+        <v>41.199999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="9">
+        <v>3.125</v>
+      </c>
+      <c r="L15" s="9">
+        <v>3.6000000000000005</v>
+      </c>
+      <c r="M15" s="9">
+        <v>3.5749999999999997</v>
+      </c>
+      <c r="N15" s="9">
+        <v>3.4333333333333331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0.1158333333333334</v>
+      </c>
+      <c r="L16" s="9">
+        <v>8.6666666666666614E-2</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0.15583333333333327</v>
+      </c>
+      <c r="N16" s="9">
+        <v>0.14969696969697308</v>
+      </c>
+    </row>
+    <row r="17" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+    </row>
+    <row r="19" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="9">
+        <v>4</v>
+      </c>
+      <c r="L19" s="9">
+        <v>4</v>
+      </c>
+      <c r="M19" s="9">
+        <v>4</v>
+      </c>
+      <c r="N19" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="9">
+        <v>11.5</v>
+      </c>
+      <c r="L20" s="9">
+        <v>14.5</v>
+      </c>
+      <c r="M20" s="9">
+        <v>15</v>
+      </c>
+      <c r="N20" s="9">
+        <v>40.999999999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="9">
+        <v>2.875</v>
+      </c>
+      <c r="L21" s="9">
+        <v>3.625</v>
+      </c>
+      <c r="M21" s="9">
+        <v>3.75</v>
+      </c>
+      <c r="N21" s="9">
+        <v>3.4166666666666661</v>
+      </c>
+    </row>
+    <row r="22" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0.1824999999999998</v>
+      </c>
+      <c r="L22" s="9">
+        <v>0.19583333333333286</v>
+      </c>
+      <c r="M22" s="9">
+        <v>9.6666666666666581E-2</v>
+      </c>
+      <c r="N22" s="9">
+        <v>0.2924242424242452</v>
+      </c>
+    </row>
+    <row r="23" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+    </row>
+    <row r="24" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+    </row>
+    <row r="25" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="9">
+        <v>8</v>
+      </c>
+      <c r="L25" s="9">
+        <v>8</v>
+      </c>
+      <c r="M25" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="9">
+        <v>24</v>
+      </c>
+      <c r="L26" s="9">
+        <v>28.900000000000002</v>
+      </c>
+      <c r="M26" s="9">
+        <v>29.299999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J27" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27" s="9">
+        <v>3</v>
+      </c>
+      <c r="L27" s="9">
+        <v>3.6125000000000003</v>
+      </c>
+      <c r="M27" s="9">
+        <v>3.6624999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J28" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="9">
+        <v>0.14571428571428516</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0.12124999999999993</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0.11696428571428563</v>
+      </c>
+    </row>
+    <row r="29" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+    </row>
+    <row r="31" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="O32" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P32" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" s="9">
+        <v>1.6666666666669272E-3</v>
+      </c>
+      <c r="L33" s="9">
+        <v>1</v>
+      </c>
+      <c r="M33" s="9">
+        <v>1.6666666666669272E-3</v>
+      </c>
+      <c r="N33" s="9">
+        <v>1.2000000000001877E-2</v>
+      </c>
+      <c r="O33" s="9">
+        <v>0.91398265748428698</v>
+      </c>
+      <c r="P33" s="9">
+        <v>4.4138734191705664</v>
+      </c>
+    </row>
+    <row r="34" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J34" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K34" s="9">
+        <v>2.1775000000000007</v>
+      </c>
+      <c r="L34" s="9">
+        <v>2</v>
+      </c>
+      <c r="M34" s="9">
+        <v>1.0887500000000003</v>
+      </c>
+      <c r="N34" s="9">
+        <v>7.839000000000004</v>
+      </c>
+      <c r="O34" s="9">
+        <v>3.559064941048024E-3</v>
+      </c>
+      <c r="P34" s="9">
+        <v>3.5545571456617879</v>
+      </c>
+    </row>
+    <row r="35" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J35" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K35" s="9">
+        <v>0.18583333333333307</v>
+      </c>
+      <c r="L35" s="9">
+        <v>2</v>
+      </c>
+      <c r="M35" s="9">
+        <v>9.2916666666666536E-2</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0.66899999999999915</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0.52450368392211755</v>
+      </c>
+      <c r="P35" s="9">
+        <v>3.5545571456617879</v>
+      </c>
+    </row>
+    <row r="36" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J36" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K36" s="9">
+        <v>2.4999999999999996</v>
+      </c>
+      <c r="L36" s="9">
+        <v>18</v>
+      </c>
+      <c r="M36" s="9">
+        <v>0.13888888888888887</v>
+      </c>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+    </row>
+    <row r="37" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+    </row>
+    <row r="38" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J38" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="11">
+        <v>4.8650000000000002</v>
+      </c>
+      <c r="L38" s="11">
+        <v>23</v>
+      </c>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>